<commit_message>
Hydroflask helper and 2 new class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8467C21F-3FFF-4B15-961B-D67292BA99FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D07284F-AFB3-4484-BD2B-9D4979261B9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20340" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
   <si>
     <t>UserName</t>
   </si>
@@ -328,6 +327,15 @@
   </si>
   <si>
     <t>oxobuyer123</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>5111005111051128</t>
+  </si>
+  <si>
+    <t>Ccmastercard</t>
   </si>
 </sst>
 </file>
@@ -388,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -404,6 +412,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -686,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU14"/>
+  <dimension ref="A1:AU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,6 +723,7 @@
     <col min="19" max="19" width="17.28515625" customWidth="1"/>
     <col min="20" max="20" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="27.28515625" customWidth="1"/>
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
@@ -987,14 +999,14 @@
     </row>
     <row r="5" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="C5" s="1"/>
       <c r="W5" t="s">
-        <v>22</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>26</v>
+        <v>100</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>101</v>
       </c>
       <c r="Y5" s="3">
         <v>2025</v>
@@ -1006,62 +1018,30 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="W6" t="s">
+        <v>22</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>2025</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S6" t="s">
-        <v>20</v>
-      </c>
-      <c r="T6" t="s">
-        <v>21</v>
-      </c>
-      <c r="U6">
-        <v>12345</v>
-      </c>
-      <c r="V6">
-        <v>9898989899</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
@@ -1077,17 +1057,18 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
-        <v>39</v>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="P7" t="s">
         <v>20</v>
@@ -1113,7 +1094,10 @@
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1126,6 +1110,15 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="L8" t="s">
         <v>39</v>
       </c>
@@ -1150,142 +1143,182 @@
       <c r="V8">
         <v>9898989899</v>
       </c>
-      <c r="AC8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE8">
-        <v>123456</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
+      <c r="L9" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" t="s">
+        <v>21</v>
+      </c>
+      <c r="U9">
+        <v>12345</v>
+      </c>
+      <c r="V9">
+        <v>9898989899</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE9">
+        <v>123456</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AI11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:47" s="8" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:47" s="8" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AJ11" s="8" t="s">
+      <c r="AJ12" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="AK11" s="8" t="s">
+      <c r="AK12" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="AL11" s="9" t="s">
+      <c r="AL12" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="AM11" s="8" t="s">
+      <c r="AM12" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="AN11" s="8" t="s">
+      <c r="AN12" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AO11" s="8" t="s">
+      <c r="AO12" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="AP11" s="8">
+      <c r="AP12" s="8">
         <v>27</v>
       </c>
-      <c r="AQ11" s="8" t="s">
+      <c r="AQ12" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AR11" s="8" t="s">
+      <c r="AR12" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AS11" s="8" t="s">
+      <c r="AS12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AT11" s="8">
+      <c r="AT12" s="8">
         <v>2</v>
       </c>
-      <c r="AU11" s="8" t="s">
+      <c r="AU12" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="W14" t="s">
+      <c r="C15" s="1"/>
+      <c r="W15" t="s">
         <v>22</v>
       </c>
-      <c r="X14" s="5" t="s">
+      <c r="X15" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="Y14" s="3">
+      <c r="Y15" s="3">
         <v>2025</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="Z15" t="s">
         <v>25</v>
       </c>
-      <c r="AB14" s="4">
+      <c r="AB15" s="4">
         <v>123</v>
       </c>
     </row>
@@ -1295,17 +1328,17 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="F4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C6" r:id="rId6" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C7" r:id="rId7" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="I7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="F3" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F12" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F13" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G13" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>

<commit_message>
Hydrofalsk O2C_E2E orders testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27172E83-564A-4789-9509-BFB4107E7671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE25090-E7EB-4DF6-ABEA-5A3355097876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -1029,7 +1029,7 @@
   <dimension ref="A1:BW36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T28" sqref="T28"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hydroflask test data, updated tes cases and helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE25090-E7EB-4DF6-ABEA-5A3355097876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7200B390-B99A-443C-BFC2-D07334B1AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="212">
   <si>
     <t>UserName</t>
   </si>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="M16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,8 +2218,8 @@
       <c r="T36" t="s">
         <v>56</v>
       </c>
-      <c r="U36">
-        <v>6492</v>
+      <c r="U36" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="V36">
         <v>989898989</v>

</xml_diff>

<commit_message>
Updated test cases,helper and test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7200B390-B99A-443C-BFC2-D07334B1AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43B5F8F-30C7-4270-9C11-2182782C8889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="213">
   <si>
     <t>UserName</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>wallingford</t>
+  </si>
+  <si>
+    <t>InvalidAddress1</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,6 +2196,38 @@
         <v>201</v>
       </c>
     </row>
+    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>212</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2</v>
+      </c>
+      <c r="P35" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>205</v>
+      </c>
+      <c r="S35" t="s">
+        <v>195</v>
+      </c>
+      <c r="T35" t="s">
+        <v>56</v>
+      </c>
+      <c r="U35" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="V35">
+        <v>989898989</v>
+      </c>
+    </row>
     <row r="36" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>202</v>

</xml_diff>

<commit_message>
Hydroflask- Order XML Magento
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
+++ b/src/test/resources/TestData/Hydroflask/HydroTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43B5F8F-30C7-4270-9C11-2182782C8889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4031C8-BF0B-460B-ABFB-18BD2E79C9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="215">
   <si>
     <t>UserName</t>
   </si>
@@ -317,9 +317,6 @@
     <t>invlidPaymentDetails</t>
   </si>
   <si>
-    <t>mahe</t>
-  </si>
-  <si>
     <t>MasterCard</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
     <t>manojk</t>
   </si>
   <si>
-    <t>b{?e\Gm=c8qDH8p@</t>
-  </si>
-  <si>
     <t>account_Enquiry</t>
   </si>
   <si>
@@ -491,9 +485,6 @@
     <t>Good products</t>
   </si>
   <si>
-    <t>Mahendra</t>
-  </si>
-  <si>
     <t>Channel</t>
   </si>
   <si>
@@ -560,12 +551,6 @@
     <t>PaypalDetails</t>
   </si>
   <si>
-    <t>mahendr.se@gmail.com</t>
-  </si>
-  <si>
-    <t>mahendr.selm@gmail.com</t>
-  </si>
-  <si>
     <t>mahendr.senium@gmail.com</t>
   </si>
   <si>
@@ -665,7 +650,28 @@
     <t>wallingford</t>
   </si>
   <si>
-    <t>InvalidAddress1</t>
+    <t>qalotuswave@gmail.com</t>
+  </si>
+  <si>
+    <t>HydroflaskQA@123</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Qatesting</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>8EHqdUqCRHXGrAE</t>
+  </si>
+  <si>
+    <t>ajith</t>
   </si>
 </sst>
 </file>
@@ -675,7 +681,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +703,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -726,7 +738,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -748,6 +760,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1029,58 +1042,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BW36"/>
+  <dimension ref="A1:BW35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="32.28515625" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="28.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
-    <col min="13" max="13" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" customWidth="1"/>
-    <col min="20" max="20" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="32.26953125" customWidth="1"/>
+    <col min="9" max="9" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="28.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" customWidth="1"/>
+    <col min="13" max="13" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1796875" customWidth="1"/>
+    <col min="15" max="15" width="18.26953125" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.26953125" customWidth="1"/>
+    <col min="20" max="20" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.26953125" customWidth="1"/>
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.7109375" customWidth="1"/>
-    <col min="37" max="37" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="21.140625" customWidth="1"/>
-    <col min="39" max="39" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="146.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.7265625" customWidth="1"/>
+    <col min="37" max="37" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.1796875" customWidth="1"/>
+    <col min="39" max="39" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="146.81640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="43.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1221,108 +1234,108 @@
         <v>81</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AW1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AY1" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="AZ1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BA1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="BD1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="BS1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="BT1" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="BU1" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="BV1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="BW1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>209</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1334,19 +1347,19 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>86</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1376,19 +1389,19 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1418,16 +1431,16 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1"/>
       <c r="W5" t="s">
+        <v>96</v>
+      </c>
+      <c r="X5" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>98</v>
       </c>
       <c r="Y5" s="3">
         <v>2025</v>
@@ -1439,7 +1452,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:75" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1460,21 +1473,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:75" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>208</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1513,26 +1526,26 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>208</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>43</v>
@@ -1565,18 +1578,18 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1623,7 +1636,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1631,7 +1644,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:75" s="8" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75" s="8" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>73</v>
       </c>
@@ -1675,7 +1688,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -1685,7 +1698,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1708,7 +1721,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:75" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -1729,26 +1742,26 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AV15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>105</v>
-      </c>
       <c r="D16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" t="s">
         <v>119</v>
       </c>
-      <c r="E16" t="s">
+      <c r="P16" t="s">
         <v>120</v>
-      </c>
-      <c r="P16" t="s">
-        <v>121</v>
       </c>
       <c r="Q16" t="s">
         <v>21</v>
@@ -1763,107 +1776,107 @@
         <v>9898989889</v>
       </c>
       <c r="AW16" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="AX16" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="AY16" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AZ16" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:74" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>204</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>205</v>
+      </c>
+      <c r="AY17" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>111</v>
       </c>
-      <c r="AW17" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX17" t="s">
-        <v>210</v>
-      </c>
-      <c r="AY17" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>112</v>
-      </c>
       <c r="AZ18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:74" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>115</v>
       </c>
       <c r="C19" s="1"/>
       <c r="W19" t="s">
+        <v>115</v>
+      </c>
+      <c r="X19" s="10" t="s">
         <v>116</v>
-      </c>
-      <c r="X19" s="10" t="s">
-        <v>117</v>
       </c>
       <c r="Y19" s="3">
         <v>2025</v>
       </c>
       <c r="Z19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB19" s="4">
         <v>1234</v>
       </c>
     </row>
-    <row r="20" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="W20" t="s">
+        <v>122</v>
+      </c>
+      <c r="X20" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="X20" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="Y20">
         <v>2025</v>
       </c>
       <c r="Z20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AB20">
         <v>342</v>
       </c>
     </row>
-    <row r="21" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>125</v>
+      </c>
+      <c r="P21" t="s">
         <v>126</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>127</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="T21" t="s">
         <v>128</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="U21" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="V21" s="4">
         <v>9898989899</v>
       </c>
     </row>
-    <row r="22" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -1872,16 +1885,16 @@
         <v>8</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="P22" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q22" t="s">
         <v>132</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="T22" t="s">
         <v>133</v>
-      </c>
-      <c r="T22" t="s">
-        <v>134</v>
       </c>
       <c r="U22">
         <v>88063</v>
@@ -1890,9 +1903,9 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="23" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -1901,47 +1914,47 @@
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="P23" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q23" t="s">
         <v>136</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="T23" t="s">
+        <v>133</v>
+      </c>
+      <c r="U23" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="T23" t="s">
-        <v>134</v>
-      </c>
-      <c r="U23" s="11" t="s">
+    </row>
+    <row r="24" spans="1:74" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="24" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="B24" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>140</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E25" t="s">
+        <v>210</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="L25" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>142</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L25" t="s">
-        <v>143</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>31</v>
@@ -1953,7 +1966,7 @@
         <v>21</v>
       </c>
       <c r="R25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="S25" t="s">
         <v>21</v>
@@ -1965,13 +1978,13 @@
         <v>9898989899</v>
       </c>
       <c r="BA25" t="s">
+        <v>143</v>
+      </c>
+      <c r="BB25" t="s">
+        <v>144</v>
+      </c>
+      <c r="BC25" t="s">
         <v>145</v>
-      </c>
-      <c r="BB25" t="s">
-        <v>146</v>
-      </c>
-      <c r="BC25" t="s">
-        <v>147</v>
       </c>
       <c r="BD25" t="s">
         <v>69</v>
@@ -1980,10 +1993,10 @@
         <v>69</v>
       </c>
       <c r="BF25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="BG25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="BH25">
         <v>9</v>
@@ -1992,7 +2005,7 @@
         <v>10</v>
       </c>
       <c r="BJ25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="BK25" s="12">
         <v>40000</v>
@@ -2007,47 +2020,47 @@
         <v>57</v>
       </c>
       <c r="BO25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="BP25">
         <v>57501</v>
       </c>
       <c r="BQ25" t="s">
+        <v>149</v>
+      </c>
+      <c r="BR25" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS25" t="s">
         <v>151</v>
       </c>
-      <c r="BR25" t="s">
-        <v>152</v>
-      </c>
-      <c r="BS25" t="s">
-        <v>153</v>
-      </c>
       <c r="BT25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="BU25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:74" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -2059,13 +2072,13 @@
         <v>2</v>
       </c>
       <c r="P27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q27" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="T27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U27">
         <v>28779</v>
@@ -2074,9 +2087,9 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="28" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -2085,13 +2098,13 @@
         <v>8</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P28" t="s">
         <v>57</v>
       </c>
       <c r="Q28" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="T28" t="s">
         <v>56</v>
@@ -2103,9 +2116,9 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="29" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -2117,13 +2130,13 @@
         <v>2</v>
       </c>
       <c r="P29" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="Q29" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="T29" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="U29">
         <v>19702</v>
@@ -2132,12 +2145,12 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="30" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D30" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -2146,13 +2159,13 @@
         <v>2</v>
       </c>
       <c r="P30" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="Q30" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="T30" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="U30">
         <v>99507</v>
@@ -2161,44 +2174,47 @@
         <v>8989898989</v>
       </c>
     </row>
-    <row r="31" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="BV31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>182</v>
+      </c>
+      <c r="BV32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>183</v>
+      </c>
+      <c r="BN33" t="s">
+        <v>212</v>
+      </c>
+      <c r="BW33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>187</v>
-      </c>
-      <c r="BV32" t="s">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>188</v>
-      </c>
-      <c r="BW33" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>200</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>212</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -2210,81 +2226,46 @@
         <v>2</v>
       </c>
       <c r="P35" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="Q35" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="S35" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="T35" t="s">
         <v>56</v>
       </c>
-      <c r="U35" s="11" t="s">
-        <v>59</v>
+      <c r="U35">
+        <v>6492</v>
       </c>
       <c r="V35">
         <v>989898989</v>
       </c>
     </row>
-    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>202</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" t="s">
-        <v>2</v>
-      </c>
-      <c r="P36" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>205</v>
-      </c>
-      <c r="S36" t="s">
-        <v>195</v>
-      </c>
-      <c r="T36" t="s">
-        <v>56</v>
-      </c>
-      <c r="U36" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="V36">
-        <v>989898989</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C8" r:id="rId3" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="I8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="AZ16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F2" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C2" r:id="rId16" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B2" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F25" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F26" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F28" r:id="rId20" xr:uid="{C22AADFC-1A71-4E22-8E4A-BA7A0A7E5477}"/>
-    <hyperlink ref="F34" r:id="rId21" xr:uid="{49D08808-F7E2-48E4-AACC-4E7FE43E8B69}"/>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="AZ16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F22" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F23" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F26" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F28" r:id="rId8" xr:uid="{C22AADFC-1A71-4E22-8E4A-BA7A0A7E5477}"/>
+    <hyperlink ref="F34" r:id="rId9" xr:uid="{49D08808-F7E2-48E4-AACC-4E7FE43E8B69}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C2" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B2" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I8" r:id="rId16" xr:uid="{7D051DC0-8CE9-4786-8201-F77682EAAB8D}"/>
+    <hyperlink ref="F3" r:id="rId17" xr:uid="{46A60F5E-D407-419C-BDAF-4AF87FE556E7}"/>
+    <hyperlink ref="F4" r:id="rId18" xr:uid="{535F6AC4-8AB8-4E3B-81D1-CA9309628366}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>